<commit_message>
added support for running in emulators such as WSA
</commit_message>
<xml_diff>
--- a/Android/Support/Notes/NET Environment.xlsx
+++ b/Android/Support/Notes/NET Environment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
   <si>
     <t>Model</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>3.18.71 Mon Mar 4 2019 14:31:59 CST</t>
+  </si>
+  <si>
+    <t>X64</t>
+  </si>
+  <si>
+    <t>5.15.104.20230927 Wed Sep 27 2023 23:05:03 UTC</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +531,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
@@ -673,33 +679,36 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -716,7 +725,7 @@
         <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -733,13 +742,10 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>45</v>
@@ -747,19 +753,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1">
-        <v>7.1</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
         <v>45</v>
@@ -776,13 +785,10 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
         <v>45</v>
@@ -790,22 +796,25 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7.1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,13 +828,10 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
         <v>46</v>
@@ -833,22 +839,25 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -862,13 +871,10 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s">
         <v>45</v>
@@ -876,22 +882,25 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -905,13 +914,10 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
         <v>46</v>
@@ -919,19 +925,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
         <v>46</v>
@@ -948,15 +957,35 @@
         <v>30</v>
       </c>
       <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated .Net Environments for android 16
</commit_message>
<xml_diff>
--- a/Android/Support/Notes/NET Environment.xlsx
+++ b/Android/Support/Notes/NET Environment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
   <si>
     <t>Model</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>5.15.104.20230927 Wed Sep 27 2023 23:05:03 UTC</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5.15.180 Thu Oct 23 2025 00:27:49 UTC</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +573,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
@@ -590,13 +596,10 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
@@ -609,11 +612,11 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
-        <v>14</v>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -630,19 +633,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,13 +662,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
@@ -670,22 +673,25 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -699,13 +705,10 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -713,22 +716,25 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -745,7 +751,7 @@
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
         <v>45</v>
@@ -762,13 +768,10 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
         <v>45</v>
@@ -776,19 +779,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
-        <v>7.1</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
         <v>45</v>
@@ -805,13 +811,10 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
         <v>45</v>
@@ -819,22 +822,25 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7.1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,13 +854,10 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
         <v>46</v>
@@ -862,22 +865,25 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -891,13 +897,10 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
         <v>45</v>
@@ -905,22 +908,25 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -934,13 +940,10 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
         <v>46</v>
@@ -948,19 +951,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
         <v>46</v>
@@ -977,15 +983,35 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>8</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>10</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>